<commit_message>
Add data files via Upload
</commit_message>
<xml_diff>
--- a/docs/analysis/chla_2.1_elk.xlsx
+++ b/docs/analysis/chla_2.1_elk.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://floridadep-my.sharepoint.com/personal/shannon_dunnigan_dep_state_fl_us/Documents/OPEN_PROJECTS/chla-nerrs-catalyst/analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dunnigan_s\OneDrive - Florida Department of Environmental Protection\OPEN_PROJECTS\chla-nerrs-catalyst\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{0012B207-F29D-4140-9823-9670A39E886E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3D4D3540-ADA2-4B2C-A341-DF0727E6B5A4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271EEFE7-47C3-4C78-8F02-D8AA4DE09831}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1878" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1878" uniqueCount="60">
   <si>
     <t>sample_no</t>
   </si>
@@ -232,6 +232,9 @@
   <si>
     <t>elksmwq083021.csv</t>
   </si>
+  <si>
+    <t>&lt;-3&gt;</t>
+  </si>
 </sst>
 </file>
 
@@ -244,11 +247,18 @@
     <numFmt numFmtId="166" formatCode="#0.0"/>
     <numFmt numFmtId="167" formatCode="#0"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -760,1771 +770,1772 @@
   </borders>
   <cellStyleXfs count="1669">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2"/>
+    <xf numFmtId="43" fontId="24" fillId="0" borderId="2" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="2"/>
-    <xf numFmtId="43" fontId="23" fillId="0" borderId="2" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="2" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="2" fontId="27" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="12" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="12" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="27" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="27" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="27" fillId="0" borderId="2" xfId="12" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="28" fillId="0" borderId="2" xfId="12" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1669">
     <cellStyle name="20% - Accent1 10" xfId="184" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -9045,7 +9056,7 @@
       <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A81" sqref="A81:A120"/>
+      <selection pane="bottomRight" activeCell="R54" sqref="R54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12698,8 +12709,8 @@
       <c r="Q33" s="17">
         <v>-3.35</v>
       </c>
-      <c r="R33" s="43" t="s">
-        <v>53</v>
+      <c r="R33" s="55" t="s">
+        <v>59</v>
       </c>
       <c r="S33" s="17">
         <v>4.92</v>
@@ -12808,8 +12819,8 @@
       <c r="Q34" s="17">
         <v>-1.94</v>
       </c>
-      <c r="R34" s="43" t="s">
-        <v>53</v>
+      <c r="R34" s="55" t="s">
+        <v>59</v>
       </c>
       <c r="S34" s="17">
         <v>5.4</v>
@@ -12918,8 +12929,8 @@
       <c r="Q35" s="17">
         <v>-0.11</v>
       </c>
-      <c r="R35" s="43" t="s">
-        <v>53</v>
+      <c r="R35" s="55" t="s">
+        <v>59</v>
       </c>
       <c r="S35" s="17">
         <v>6.01</v>
@@ -13138,8 +13149,8 @@
       <c r="Q37" s="17">
         <v>-0.03</v>
       </c>
-      <c r="R37" s="43" t="s">
-        <v>53</v>
+      <c r="R37" s="55" t="s">
+        <v>59</v>
       </c>
       <c r="S37" s="17">
         <v>6.04</v>
@@ -13248,8 +13259,8 @@
       <c r="Q38" s="17">
         <v>-2.91</v>
       </c>
-      <c r="R38" s="43" t="s">
-        <v>53</v>
+      <c r="R38" s="55" t="s">
+        <v>59</v>
       </c>
       <c r="S38" s="17">
         <v>5.07</v>
@@ -13358,8 +13369,8 @@
       <c r="Q39" s="17">
         <v>-7.3</v>
       </c>
-      <c r="R39" s="43" t="s">
-        <v>53</v>
+      <c r="R39" s="55" t="s">
+        <v>59</v>
       </c>
       <c r="S39" s="17">
         <v>3.6</v>
@@ -13468,8 +13479,8 @@
       <c r="Q40" s="17">
         <v>-5.07</v>
       </c>
-      <c r="R40" s="43" t="s">
-        <v>53</v>
+      <c r="R40" s="55" t="s">
+        <v>59</v>
       </c>
       <c r="S40" s="17">
         <v>4.3499999999999996</v>
@@ -13798,8 +13809,8 @@
       <c r="Q43" s="17">
         <v>-10.61</v>
       </c>
-      <c r="R43" s="43" t="s">
-        <v>53</v>
+      <c r="R43" s="55" t="s">
+        <v>59</v>
       </c>
       <c r="S43" s="17">
         <v>2.4900000000000002</v>
@@ -13908,8 +13919,8 @@
       <c r="Q44" s="17">
         <v>-4.1399999999999997</v>
       </c>
-      <c r="R44" s="43" t="s">
-        <v>53</v>
+      <c r="R44" s="55" t="s">
+        <v>59</v>
       </c>
       <c r="S44" s="17">
         <v>4.66</v>
@@ -14458,8 +14469,8 @@
       <c r="Q49" s="17">
         <v>-1.82</v>
       </c>
-      <c r="R49" s="43" t="s">
-        <v>53</v>
+      <c r="R49" s="55" t="s">
+        <v>59</v>
       </c>
       <c r="S49" s="17">
         <v>5.44</v>
@@ -14568,8 +14579,8 @@
       <c r="Q50" s="17">
         <v>-7.81</v>
       </c>
-      <c r="R50" s="43" t="s">
-        <v>53</v>
+      <c r="R50" s="55" t="s">
+        <v>59</v>
       </c>
       <c r="S50" s="17">
         <v>3.43</v>
@@ -14678,8 +14689,8 @@
       <c r="Q51" s="17">
         <v>-2.2200000000000002</v>
       </c>
-      <c r="R51" s="43" t="s">
-        <v>53</v>
+      <c r="R51" s="55" t="s">
+        <v>59</v>
       </c>
       <c r="S51" s="17">
         <v>5.3</v>
@@ -15008,8 +15019,8 @@
       <c r="Q54" s="17">
         <v>-0.24</v>
       </c>
-      <c r="R54" s="43" t="s">
-        <v>53</v>
+      <c r="R54" s="55" t="s">
+        <v>59</v>
       </c>
       <c r="S54" s="17">
         <v>5.97</v>

</xml_diff>